<commit_message>
sao luu du lieu ngay 02/06/2025
</commit_message>
<xml_diff>
--- a/APP_KHAI_BAO_LUU_TRU_2/DU_LIEU_KHAI_BAO.xlsx
+++ b/APP_KHAI_BAO_LUU_TRU_2/DU_LIEU_KHAI_BAO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796070A3-0155-4757-A839-AC5A33DE65A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DFFFBAA-EEA0-4A01-AF20-19D3B0040231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F7DBCA89-BBD2-4D0C-8CEF-0E38599E368D}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C1FB65B3-53A1-487D-832C-63068A3A0ED2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="19">
   <si>
     <t>Số giấy tờ</t>
   </si>
@@ -74,25 +74,25 @@
     <t>Ảnh mặt sau</t>
   </si>
   <si>
-    <t>Ngô Xuân Trọng</t>
+    <t>Nguyễn Văn Hoài</t>
   </si>
   <si>
     <t>Nam</t>
   </si>
   <si>
-    <t>28/08/2005</t>
-  </si>
-  <si>
-    <t>Ấp Phụng Thạnh, Thạnh Tiến, Vĩnh Thạnh, Cần Thơ</t>
-  </si>
-  <si>
-    <t>13/05/2021</t>
+    <t>23/02/2003</t>
+  </si>
+  <si>
+    <t>Khu Phố 4, An Thới, TP. Phú Quốc, Kiên Giang</t>
   </si>
   <si>
     <t>CCCD</t>
   </si>
   <si>
     <t>Phòng 3 nhà cũ</t>
+  </si>
+  <si>
+    <t>Phòng 4 nhà cũ</t>
   </si>
 </sst>
 </file>
@@ -150,7 +150,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -184,6 +184,21 @@
         <color auto="1"/>
       </top>
       <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -193,7 +208,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -201,10 +216,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="22" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -541,21 +571,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B58D0A37-F5C1-4675-A6EB-2702F37B217A}">
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0D2A2A6-B2C0-47E2-AB8E-06A4FAC001A6}">
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
@@ -604,9 +632,11 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>92205005260</v>
-      </c>
-      <c r="B2" s="2"/>
+        <v>91203001544</v>
+      </c>
+      <c r="B2" s="2">
+        <v>371987447</v>
+      </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
@@ -619,24 +649,424 @@
       <c r="F2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="3">
+        <v>44381</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="4">
+        <v>45694.479907407411</v>
+      </c>
+      <c r="K2" s="5" t="str">
+        <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU_2\Anh_CCCD_da_khai_bao\mat_truoc_20250602_113104.jpg", "Ảnh mặt trước")</f>
+        <v>Ảnh mặt trước</v>
+      </c>
+      <c r="L2" s="5" t="str">
+        <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU_2\Anh_CCCD_da_khai_bao\mat_sau_20250602_113104.jpg", "Ảnh mặt sau")</f>
+        <v>Ảnh mặt sau</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>91203001544</v>
+      </c>
+      <c r="B3" s="2">
+        <v>371987447</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="3">
+        <v>44381</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="4">
+        <v>45694.481724537036</v>
+      </c>
+      <c r="K3" s="5" t="str">
+        <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU_2\Anh_CCCD_da_khai_bao\mat_truoc_20250602_113340.jpg", "Ảnh mặt trước")</f>
+        <v>Ảnh mặt trước</v>
+      </c>
+      <c r="L3" s="5" t="str">
+        <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU_2\Anh_CCCD_da_khai_bao\mat_sau_20250602_113340.jpg", "Ảnh mặt sau")</f>
+        <v>Ảnh mặt sau</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>91203001544</v>
+      </c>
+      <c r="B4" s="2">
+        <v>371987447</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="3">
+        <v>44381</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="4">
+        <v>45694.483067129629</v>
+      </c>
+      <c r="K4" s="5" t="str">
+        <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU_2\Anh_CCCD_da_khai_bao\mat_truoc_20250602_113537.jpg", "Ảnh mặt trước")</f>
+        <v>Ảnh mặt trước</v>
+      </c>
+      <c r="L4" s="5" t="str">
+        <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU_2\Anh_CCCD_da_khai_bao\mat_sau_20250602_113537.jpg", "Ảnh mặt sau")</f>
+        <v>Ảnh mặt sau</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>91203001544</v>
+      </c>
+      <c r="B5" s="2">
+        <v>371987447</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="3">
+        <v>44381</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="4">
+        <v>45694.484884259262</v>
+      </c>
+      <c r="K5" s="5" t="str">
+        <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU_2\Anh_CCCD_da_khai_bao\mat_truoc_20250602_113814.jpg", "Ảnh mặt trước")</f>
+        <v>Ảnh mặt trước</v>
+      </c>
+      <c r="L5" s="5" t="str">
+        <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU_2\Anh_CCCD_da_khai_bao\mat_sau_20250602_113814.jpg", "Ảnh mặt sau")</f>
+        <v>Ảnh mặt sau</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>91203001544</v>
+      </c>
+      <c r="B6" s="2">
+        <v>371987447</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="3">
+        <v>44381</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="4">
+        <v>45694.485289351855</v>
+      </c>
+      <c r="K6" s="5" t="str">
+        <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU_2\Anh_CCCD_da_khai_bao\mat_truoc_20250602_113849.jpg", "Ảnh mặt trước")</f>
+        <v>Ảnh mặt trước</v>
+      </c>
+      <c r="L6" s="5" t="str">
+        <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU_2\Anh_CCCD_da_khai_bao\mat_sau_20250602_113849.jpg", "Ảnh mặt sau")</f>
+        <v>Ảnh mặt sau</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>91203001544</v>
+      </c>
+      <c r="B7" s="2">
+        <v>371987447</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="3">
+        <v>44381</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="4">
+        <v>45694.486400462964</v>
+      </c>
+      <c r="K7" s="5" t="str">
+        <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU_2\Anh_CCCD_da_khai_bao\mat_truoc_20250602_114025.jpg", "Ảnh mặt trước")</f>
+        <v>Ảnh mặt trước</v>
+      </c>
+      <c r="L7" s="5" t="str">
+        <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU_2\Anh_CCCD_da_khai_bao\mat_sau_20250602_114025.jpg", "Ảnh mặt sau")</f>
+        <v>Ảnh mặt sau</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>91203001544</v>
+      </c>
+      <c r="B8" s="2">
+        <v>371987447</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="3">
+        <v>44381</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="3">
-        <v>45663.84165509259</v>
-      </c>
-      <c r="K2" s="4" t="str">
-        <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU_2\Anh_CCCD_da_khai_bao\z6659098829266_d6ca5a653cecaa34d5e450ae9f10d090.jpg", "Ảnh mặt trước")</f>
+      <c r="J8" s="4">
+        <v>45694.486956018518</v>
+      </c>
+      <c r="K8" s="5" t="str">
+        <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU_2\Anh_CCCD_da_khai_bao\mat_truoc_20250602_114113.jpg", "Ảnh mặt trước")</f>
         <v>Ảnh mặt trước</v>
       </c>
-      <c r="L2" s="4" t="str">
-        <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU_2\Anh_CCCD_da_khai_bao\z6659098735032_dd8afed50c6c71bb10b6183cd5c28e8f.jpg", "Ảnh mặt sau")</f>
+      <c r="L8" s="5" t="str">
+        <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU_2\Anh_CCCD_da_khai_bao\mat_sau_20250602_114113.jpg", "Ảnh mặt sau")</f>
+        <v>Ảnh mặt sau</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>91203001544</v>
+      </c>
+      <c r="B9" s="2">
+        <v>371987447</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="3">
+        <v>44381</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="4">
+        <v>45694.488530092596</v>
+      </c>
+      <c r="K9" s="5" t="str">
+        <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU_2\Anh_CCCD_da_khai_bao\mat_truoc_20250602_114329.jpg", "Ảnh mặt trước")</f>
+        <v>Ảnh mặt trước</v>
+      </c>
+      <c r="L9" s="5" t="str">
+        <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU_2\Anh_CCCD_da_khai_bao\mat_sau_20250602_114329.jpg", "Ảnh mặt sau")</f>
+        <v>Ảnh mặt sau</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>91203001544</v>
+      </c>
+      <c r="B10" s="2">
+        <v>371987447</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="3">
+        <v>44381</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="4">
+        <v>45694.489305555559</v>
+      </c>
+      <c r="K10" s="5" t="str">
+        <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU_2\Anh_CCCD_da_khai_bao\mat_truoc_20250602_114436.jpg", "Ảnh mặt trước")</f>
+        <v>Ảnh mặt trước</v>
+      </c>
+      <c r="L10" s="5" t="str">
+        <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU_2\Anh_CCCD_da_khai_bao\mat_sau_20250602_114436.jpg", "Ảnh mặt sau")</f>
+        <v>Ảnh mặt sau</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>91203001544</v>
+      </c>
+      <c r="B11" s="2">
+        <v>371987447</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="3">
+        <v>44381</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="4">
+        <v>45694.49255787037</v>
+      </c>
+      <c r="K11" s="5" t="str">
+        <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU_2\Anh_CCCD_da_khai_bao\mat_truoc_20250602_114917.jpg", "Ảnh mặt trước")</f>
+        <v>Ảnh mặt trước</v>
+      </c>
+      <c r="L11" s="5" t="str">
+        <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU_2\Anh_CCCD_da_khai_bao\mat_sau_20250602_114917.jpg", "Ảnh mặt sau")</f>
+        <v>Ảnh mặt sau</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>91203001544</v>
+      </c>
+      <c r="B12" s="6">
+        <v>371987447</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="7">
+        <v>44381</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="8">
+        <v>45694.493321759262</v>
+      </c>
+      <c r="K12" s="9" t="str">
+        <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU_2\Anh_CCCD_da_khai_bao\mat_truoc_20250602_115023.jpg", "Ảnh mặt trước")</f>
+        <v>Ảnh mặt trước</v>
+      </c>
+      <c r="L12" s="9" t="str">
+        <f>HYPERLINK("d:\QUAN LY NHA NGHI\APP_KHAI_BAO_LUU_TRU_2\Anh_CCCD_da_khai_bao\mat_sau_20250602_115023.jpg", "Ảnh mặt sau")</f>
         <v>Ảnh mặt sau</v>
       </c>
     </row>

</xml_diff>